<commit_message>
a big change /sub page
</commit_message>
<xml_diff>
--- a/chinaproject/资料/Property management service.xlsx
+++ b/chinaproject/资料/Property management service.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16927"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="27750" windowHeight="13665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>Items</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Yard services</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
   <si>
     <t>Emergency services</t>
@@ -76,25 +79,375 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -102,26 +455,311 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="50">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="50">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -168,7 +806,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,26 +839,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,23 +874,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,19 +1049,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -473,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -503,7 +1108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -511,7 +1116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -519,7 +1124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -527,12 +1132,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -540,7 +1145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -548,7 +1153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -556,12 +1161,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -569,12 +1174,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -582,10 +1190,11 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
a big change 5/22
</commit_message>
<xml_diff>
--- a/chinaproject/资料/Property management service.xlsx
+++ b/chinaproject/资料/Property management service.xlsx
@@ -81,12 +81,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,22 +95,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -125,6 +127,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -132,76 +165,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,17 +203,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,21 +234,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,12 +248,138 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -280,25 +392,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,49 +410,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,79 +428,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,45 +439,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -506,6 +453,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,11 +481,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,160 +515,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1054,7 +1041,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1093,7 +1080,7 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1104,7 +1091,7 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1181,7 +1168,7 @@
       <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="S17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1194,6 +1181,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="http://jbutlerpropertymgmt1-px.rtrk.com/services.htm"/>
+    <hyperlink ref="C5" r:id="rId2" display="http://www.propertymanagementlowell.com/condo-management.html"/>
+  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>